<commit_message>
Actualización de prompt para obtener el nit de comprador real
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -524,6 +524,717 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>106307649</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MENDOZA CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>MENDOZA S CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MENDOZA S CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>53492265</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5405.00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16693949</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>MENOOZA S CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>16693949</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>16693949</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>53492575</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MENDOZA S CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MENDOZA S CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>53492565</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>5405.0</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>MENOOZA S CAR AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28"/>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>53492765</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>405.0</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>588.75</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2149662922</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Mendoza Car Audio</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>